<commit_message>
Update DD, add samples
</commit_message>
<xml_diff>
--- a/Envizi-SCI Data Dictionary (simplified).xlsx
+++ b/Envizi-SCI Data Dictionary (simplified).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\903106897\Box\Sustainability Platform\2.4 Products - implementation\5. Content drafts\5. Configuring\E-SCI-data-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4BC5C4-1151-4EE0-A069-6711D1537DF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D3BA35-0682-4BEC-BBF1-CCE11FC6ADFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="2955" windowWidth="29220" windowHeight="22410" tabRatio="763" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6675" yWindow="2355" windowWidth="33540" windowHeight="24495" tabRatio="763" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data summary" sheetId="31" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="320">
   <si>
     <t>Composite</t>
   </si>
@@ -345,9 +345,6 @@
     <t>City</t>
   </si>
   <si>
-    <t>Guangdong Sheng</t>
-  </si>
-  <si>
     <t>postalCode</t>
   </si>
   <si>
@@ -483,9 +480,6 @@
     <t>IBM SHENZHEN</t>
   </si>
   <si>
-    <t>China</t>
-  </si>
-  <si>
     <t>coordinates</t>
   </si>
   <si>
@@ -576,9 +570,6 @@
     <t>secondaryIdentifier</t>
   </si>
   <si>
-    <t>USA</t>
-  </si>
-  <si>
     <t>Unique identifier for the contact.</t>
   </si>
   <si>
@@ -616,9 +607,6 @@
   </si>
   <si>
     <t>INBOUND, OUTBOUND, TRANSFER</t>
-  </si>
-  <si>
-    <t>ORGANIZATION, CUSTOMER, SUPPLIER, STORE</t>
   </si>
   <si>
     <t>Street address line one.</t>
@@ -1007,6 +995,15 @@
   </si>
   <si>
     <t>12A3456</t>
+  </si>
+  <si>
+    <t>Shenzhen</t>
+  </si>
+  <si>
+    <t>CHN</t>
+  </si>
+  <si>
+    <t>ORGANIZATION, CUSTOMER, SUPPLIER</t>
   </si>
 </sst>
 </file>
@@ -1416,7 +1413,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="17" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1639,6 +1636,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="23">
     <cellStyle name="20% - Accent1 2" xfId="15" xr:uid="{308D2E93-E68C-4D82-A3FA-122A21785EC1}"/>
@@ -2902,7 +2902,7 @@
   <sheetData>
     <row r="1" spans="2:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="82" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C1" s="83"/>
       <c r="D1" s="83"/>
@@ -2912,16 +2912,16 @@
     <row r="2" spans="2:6" s="89" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="86"/>
       <c r="C2" s="87" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="D2" s="87" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="E2" s="88" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="F2" s="88" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2929,16 +2929,16 @@
         <v>32</v>
       </c>
       <c r="C3" s="91" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D3" s="91" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="E3" s="92" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="F3" s="92" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2946,33 +2946,33 @@
         <v>76</v>
       </c>
       <c r="C4" s="94" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="D4" s="94" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="E4" s="95" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="F4" s="95" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="93" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C5" s="94" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D5" s="94" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="E5" s="95" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="F5" s="95" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2980,38 +2980,38 @@
         <v>33</v>
       </c>
       <c r="C6" s="94" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="D6" s="94" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="E6" s="95" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="F6" s="95" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="93" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C7" s="94" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="D7" s="94" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="E7" s="95" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="F7" s="95" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="82" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C8" s="83"/>
       <c r="D8" s="83"/>
@@ -3021,16 +3021,16 @@
     <row r="9" spans="2:6" s="89" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="86"/>
       <c r="C9" s="87" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="D9" s="87" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="E9" s="88" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="F9" s="88" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3038,16 +3038,16 @@
         <v>7</v>
       </c>
       <c r="C10" s="91" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="D10" s="91" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="E10" s="92" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="F10" s="92" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3055,21 +3055,21 @@
         <v>68</v>
       </c>
       <c r="C11" s="94" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D11" s="94" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="E11" s="95" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="F11" s="95" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="96" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C12" s="83"/>
       <c r="D12" s="83"/>
@@ -3079,84 +3079,84 @@
     <row r="13" spans="2:6" s="89" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="86"/>
       <c r="C13" s="87" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="D13" s="87" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="E13" s="88" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="F13" s="88" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="93" t="s">
+        <v>297</v>
+      </c>
+      <c r="C14" s="94" t="s">
+        <v>298</v>
+      </c>
+      <c r="D14" s="94" t="s">
+        <v>299</v>
+      </c>
+      <c r="E14" s="95" t="s">
+        <v>300</v>
+      </c>
+      <c r="F14" s="95" t="s">
         <v>301</v>
-      </c>
-      <c r="C14" s="94" t="s">
-        <v>302</v>
-      </c>
-      <c r="D14" s="94" t="s">
-        <v>303</v>
-      </c>
-      <c r="E14" s="95" t="s">
-        <v>304</v>
-      </c>
-      <c r="F14" s="95" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="93" t="s">
+        <v>302</v>
+      </c>
+      <c r="C15" s="94" t="s">
+        <v>303</v>
+      </c>
+      <c r="D15" s="94" t="s">
+        <v>304</v>
+      </c>
+      <c r="E15" s="95" t="s">
+        <v>305</v>
+      </c>
+      <c r="F15" s="95" t="s">
         <v>306</v>
-      </c>
-      <c r="C15" s="94" t="s">
-        <v>307</v>
-      </c>
-      <c r="D15" s="94" t="s">
-        <v>308</v>
-      </c>
-      <c r="E15" s="95" t="s">
-        <v>309</v>
-      </c>
-      <c r="F15" s="95" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="90" t="s">
+        <v>307</v>
+      </c>
+      <c r="C16" s="91" t="s">
+        <v>308</v>
+      </c>
+      <c r="D16" s="91" t="s">
+        <v>309</v>
+      </c>
+      <c r="E16" s="92" t="s">
+        <v>310</v>
+      </c>
+      <c r="F16" s="92" t="s">
         <v>311</v>
-      </c>
-      <c r="C16" s="91" t="s">
-        <v>312</v>
-      </c>
-      <c r="D16" s="91" t="s">
-        <v>313</v>
-      </c>
-      <c r="E16" s="92" t="s">
-        <v>314</v>
-      </c>
-      <c r="F16" s="92" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="90" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C17" s="91" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D17" s="91" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="E17" s="92" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="F17" s="92" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -3169,8 +3169,8 @@
   <dimension ref="A1:K89"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F40" sqref="F40"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3194,13 +3194,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -3247,23 +3247,23 @@
         <v>8</v>
       </c>
       <c r="E3" s="33" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F3" s="73" t="s">
+        <v>127</v>
+      </c>
+      <c r="G3" s="73" t="s">
         <v>128</v>
       </c>
-      <c r="G3" s="73" t="s">
-        <v>129</v>
-      </c>
       <c r="H3" s="57" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="I3" s="74" t="s">
         <v>11</v>
       </c>
       <c r="J3" s="74"/>
       <c r="K3" s="27" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -3279,23 +3279,23 @@
         <v>14</v>
       </c>
       <c r="E4" s="33" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F4" s="62" t="s">
+        <v>129</v>
+      </c>
+      <c r="G4" s="62" t="s">
         <v>130</v>
       </c>
-      <c r="G4" s="62" t="s">
-        <v>131</v>
-      </c>
       <c r="H4" s="63" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I4" s="64" t="s">
         <v>11</v>
       </c>
       <c r="J4" s="64"/>
       <c r="K4" s="70" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -3311,25 +3311,25 @@
         <v>18</v>
       </c>
       <c r="E5" s="33" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F5" s="40" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G5" s="40" t="s">
         <v>95</v>
       </c>
       <c r="H5" s="75" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I5" s="40" t="s">
         <v>22</v>
       </c>
       <c r="J5" s="40" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="K5" s="70" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -3345,25 +3345,25 @@
         <v>18</v>
       </c>
       <c r="E6" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F6" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="G6" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="G6" s="40" t="s">
+      <c r="H6" s="75" t="s">
         <v>134</v>
-      </c>
-      <c r="H6" s="75" t="s">
-        <v>135</v>
       </c>
       <c r="I6" s="40" t="s">
         <v>22</v>
       </c>
       <c r="J6" s="40" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="K6" s="70" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -3379,13 +3379,13 @@
         <v>18</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F7" s="40" t="s">
+        <v>135</v>
+      </c>
+      <c r="G7" s="40" t="s">
         <v>136</v>
-      </c>
-      <c r="G7" s="40" t="s">
-        <v>137</v>
       </c>
       <c r="H7" s="75">
         <v>7000</v>
@@ -3394,10 +3394,10 @@
         <v>22</v>
       </c>
       <c r="J7" s="40" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="K7" s="70" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -3413,25 +3413,25 @@
         <v>18</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F8" s="40" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G8" s="40" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H8" s="75" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="I8" s="40" t="s">
         <v>22</v>
       </c>
       <c r="J8" s="40" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="K8" s="27" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -3447,7 +3447,7 @@
         <v>34</v>
       </c>
       <c r="E9" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F9" s="67" t="s">
         <v>77</v>
@@ -3463,7 +3463,7 @@
       </c>
       <c r="J9" s="69"/>
       <c r="K9" s="27" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -3479,7 +3479,7 @@
         <v>50</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F10" s="67" t="s">
         <v>83</v>
@@ -3495,7 +3495,7 @@
       </c>
       <c r="J10" s="69"/>
       <c r="K10" s="27" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -3511,7 +3511,7 @@
         <v>50</v>
       </c>
       <c r="E11" s="33" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F11" s="67" t="s">
         <v>84</v>
@@ -3527,7 +3527,7 @@
       </c>
       <c r="J11" s="69"/>
       <c r="K11" s="46" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -3543,13 +3543,13 @@
         <v>50</v>
       </c>
       <c r="E12" s="76" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F12" s="67" t="s">
+        <v>137</v>
+      </c>
+      <c r="G12" s="67" t="s">
         <v>138</v>
-      </c>
-      <c r="G12" s="67" t="s">
-        <v>139</v>
       </c>
       <c r="H12" s="68" t="s">
         <v>56</v>
@@ -3559,7 +3559,7 @@
       </c>
       <c r="J12" s="69"/>
       <c r="K12" s="46" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -3575,23 +3575,23 @@
         <v>50</v>
       </c>
       <c r="E13" s="76" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F13" s="70" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G13" s="70" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H13" s="98" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="I13" s="99" t="s">
         <v>53</v>
       </c>
       <c r="J13" s="99"/>
       <c r="K13" s="27" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -3607,23 +3607,23 @@
         <v>50</v>
       </c>
       <c r="E14" s="76" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F14" s="70" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G14" s="70" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H14" s="98" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="I14" s="99" t="s">
         <v>53</v>
       </c>
       <c r="J14" s="99"/>
       <c r="K14" s="46" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -3639,7 +3639,7 @@
         <v>67</v>
       </c>
       <c r="E15" s="33" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F15" s="67" t="s">
         <v>93</v>
@@ -3655,7 +3655,7 @@
       </c>
       <c r="J15" s="69"/>
       <c r="K15" s="70" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -3671,7 +3671,7 @@
         <v>67</v>
       </c>
       <c r="E16" s="33" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F16" s="67" t="s">
         <v>87</v>
@@ -3680,14 +3680,14 @@
         <v>6</v>
       </c>
       <c r="H16" s="68" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I16" s="69" t="s">
         <v>11</v>
       </c>
       <c r="J16" s="69"/>
       <c r="K16" s="70" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -3710,29 +3710,29 @@
         <v>Catalog.levelType</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D18" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E18" s="33" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F18" s="73" t="s">
+        <v>117</v>
+      </c>
+      <c r="G18" s="73" t="s">
         <v>118</v>
       </c>
-      <c r="G18" s="73" t="s">
+      <c r="H18" s="57" t="s">
         <v>119</v>
-      </c>
-      <c r="H18" s="57" t="s">
-        <v>120</v>
       </c>
       <c r="I18" s="74" t="s">
         <v>11</v>
       </c>
       <c r="J18" s="74"/>
       <c r="K18" s="27" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -3742,29 +3742,29 @@
         <v>Catalog.code</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D19" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F19" s="73" t="s">
+        <v>120</v>
+      </c>
+      <c r="G19" s="73" t="s">
         <v>121</v>
       </c>
-      <c r="G19" s="73" t="s">
+      <c r="H19" s="57" t="s">
         <v>122</v>
-      </c>
-      <c r="H19" s="57" t="s">
-        <v>123</v>
       </c>
       <c r="I19" s="74" t="s">
         <v>11</v>
       </c>
       <c r="J19" s="74"/>
       <c r="K19" s="70" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -3774,29 +3774,29 @@
         <v>Catalog.catalogType</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D20" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E20" s="33" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F20" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="G20" s="73" t="s">
         <v>124</v>
       </c>
-      <c r="G20" s="73" t="s">
+      <c r="H20" s="57" t="s">
         <v>125</v>
-      </c>
-      <c r="H20" s="57" t="s">
-        <v>126</v>
       </c>
       <c r="I20" s="74" t="s">
         <v>11</v>
       </c>
       <c r="J20" s="74"/>
       <c r="K20" s="27" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -3806,31 +3806,31 @@
         <v>Catalog.emissionsFactorGroup.factorCode</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D21" s="37" t="s">
         <v>18</v>
       </c>
       <c r="E21" s="33" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F21" s="40" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="G21" s="38" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="H21" s="39" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="I21" s="38" t="s">
         <v>22</v>
       </c>
       <c r="J21" s="40" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="K21" s="27" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -3840,13 +3840,13 @@
         <v>Catalog.name</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D22" s="66" t="s">
         <v>67</v>
       </c>
       <c r="E22" s="33" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F22" s="67" t="s">
         <v>93</v>
@@ -3855,14 +3855,14 @@
         <v>94</v>
       </c>
       <c r="H22" s="68" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I22" s="69" t="s">
         <v>11</v>
       </c>
       <c r="J22" s="69"/>
       <c r="K22" s="70" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="23" spans="1:11" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -3872,13 +3872,13 @@
         <v>Catalog.description</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D23" s="66" t="s">
         <v>67</v>
       </c>
       <c r="E23" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F23" s="67" t="s">
         <v>87</v>
@@ -3887,14 +3887,14 @@
         <v>6</v>
       </c>
       <c r="H23" s="68" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I23" s="69" t="s">
         <v>11</v>
       </c>
       <c r="J23" s="69"/>
       <c r="K23" s="27" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="24" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3904,19 +3904,19 @@
         <v>Catalog.currentYearEmissionsTarget</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D24" s="49" t="s">
         <v>50</v>
       </c>
       <c r="E24" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F24" s="71" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G24" s="71" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H24" s="72">
         <v>159.88</v>
@@ -3926,7 +3926,7 @@
       </c>
       <c r="J24" s="71"/>
       <c r="K24" s="65" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -3955,10 +3955,10 @@
         <v>8</v>
       </c>
       <c r="E26" s="33" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F26" s="24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G26" s="24" t="s">
         <v>92</v>
@@ -3971,7 +3971,7 @@
       </c>
       <c r="J26" s="26"/>
       <c r="K26" s="27" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -3987,23 +3987,23 @@
         <v>14</v>
       </c>
       <c r="E27" s="33" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F27" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="G27" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="G27" s="34" t="s">
-        <v>143</v>
-      </c>
       <c r="H27" s="35" t="s">
-        <v>192</v>
+        <v>319</v>
       </c>
       <c r="I27" s="36" t="s">
         <v>11</v>
       </c>
       <c r="J27" s="36"/>
       <c r="K27" s="27" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -4019,23 +4019,23 @@
         <v>67</v>
       </c>
       <c r="E28" s="33" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F28" s="67" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G28" s="67" t="s">
         <v>94</v>
       </c>
       <c r="H28" s="68" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I28" s="69" t="s">
         <v>11</v>
       </c>
       <c r="J28" s="69"/>
       <c r="K28" s="70" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -4051,7 +4051,7 @@
         <v>67</v>
       </c>
       <c r="E29" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F29" s="43" t="s">
         <v>96</v>
@@ -4067,7 +4067,7 @@
       </c>
       <c r="J29" s="77"/>
       <c r="K29" s="27" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -4083,7 +4083,7 @@
         <v>67</v>
       </c>
       <c r="E30" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F30" s="43" t="s">
         <v>99</v>
@@ -4091,15 +4091,15 @@
       <c r="G30" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="H30" s="44" t="s">
-        <v>101</v>
+      <c r="H30" s="100" t="s">
+        <v>317</v>
       </c>
       <c r="I30" s="45" t="s">
         <v>11</v>
       </c>
       <c r="J30" s="45"/>
       <c r="K30" s="46" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -4115,13 +4115,13 @@
         <v>67</v>
       </c>
       <c r="E31" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F31" s="43" t="s">
+        <v>101</v>
+      </c>
+      <c r="G31" s="43" t="s">
         <v>102</v>
-      </c>
-      <c r="G31" s="43" t="s">
-        <v>103</v>
       </c>
       <c r="H31" s="44">
         <v>518057</v>
@@ -4131,7 +4131,7 @@
       </c>
       <c r="J31" s="45"/>
       <c r="K31" s="46" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="32" spans="1:11" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -4147,23 +4147,23 @@
         <v>67</v>
       </c>
       <c r="E32" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F32" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="G32" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="G32" s="43" t="s">
+      <c r="H32" s="44" t="s">
         <v>105</v>
-      </c>
-      <c r="H32" s="44" t="s">
-        <v>106</v>
       </c>
       <c r="I32" s="45" t="s">
         <v>11</v>
       </c>
       <c r="J32" s="45"/>
       <c r="K32" s="46" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="33" spans="1:11" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -4179,23 +4179,23 @@
         <v>67</v>
       </c>
       <c r="E33" s="33" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F33" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="G33" s="43" t="s">
         <v>107</v>
       </c>
-      <c r="G33" s="43" t="s">
-        <v>108</v>
-      </c>
-      <c r="H33" s="44" t="s">
-        <v>147</v>
+      <c r="H33" s="100" t="s">
+        <v>318</v>
       </c>
       <c r="I33" s="45" t="s">
         <v>11</v>
       </c>
       <c r="J33" s="45"/>
       <c r="K33" s="27" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -4211,23 +4211,23 @@
         <v>67</v>
       </c>
       <c r="E34" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F34" s="71" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G34" s="71" t="s">
-        <v>176</v>
-      </c>
-      <c r="H34" s="72" t="s">
-        <v>178</v>
+        <v>174</v>
+      </c>
+      <c r="H34" s="100" t="s">
+        <v>30</v>
       </c>
       <c r="I34" s="71" t="s">
         <v>11</v>
       </c>
       <c r="J34" s="71"/>
       <c r="K34" s="65" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -4243,13 +4243,13 @@
         <v>67</v>
       </c>
       <c r="E35" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F35" s="43" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G35" s="43" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H35" s="44" t="s">
         <v>88</v>
@@ -4259,7 +4259,7 @@
       </c>
       <c r="J35" s="45"/>
       <c r="K35" s="46" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -4288,23 +4288,23 @@
         <v>8</v>
       </c>
       <c r="E37" s="33" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F37" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="G37" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="G37" s="24" t="s">
+      <c r="H37" s="57" t="s">
         <v>110</v>
-      </c>
-      <c r="H37" s="57" t="s">
-        <v>111</v>
       </c>
       <c r="I37" s="26" t="s">
         <v>11</v>
       </c>
       <c r="J37" s="26"/>
       <c r="K37" s="27" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -4320,7 +4320,7 @@
         <v>18</v>
       </c>
       <c r="E38" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F38" s="58" t="s">
         <v>91</v>
@@ -4329,16 +4329,16 @@
         <v>92</v>
       </c>
       <c r="H38" s="59" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I38" s="60" t="s">
         <v>22</v>
       </c>
       <c r="J38" s="41" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="K38" s="27" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -4354,23 +4354,23 @@
         <v>14</v>
       </c>
       <c r="E39" s="23" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F39" s="62" t="s">
+        <v>112</v>
+      </c>
+      <c r="G39" s="62" t="s">
         <v>113</v>
       </c>
-      <c r="G39" s="62" t="s">
-        <v>114</v>
-      </c>
       <c r="H39" s="63" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="I39" s="64" t="s">
         <v>11</v>
       </c>
       <c r="J39" s="64"/>
       <c r="K39" s="27" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -4386,25 +4386,25 @@
         <v>18</v>
       </c>
       <c r="E40" s="33" t="s">
+        <v>259</v>
+      </c>
+      <c r="F40" s="38" t="s">
+        <v>262</v>
+      </c>
+      <c r="G40" s="38" t="s">
+        <v>143</v>
+      </c>
+      <c r="H40" s="39" t="s">
         <v>263</v>
-      </c>
-      <c r="F40" s="38" t="s">
-        <v>266</v>
-      </c>
-      <c r="G40" s="38" t="s">
-        <v>144</v>
-      </c>
-      <c r="H40" s="39" t="s">
-        <v>267</v>
       </c>
       <c r="I40" s="38" t="s">
         <v>22</v>
       </c>
       <c r="J40" s="38" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="K40" s="65" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -4420,23 +4420,23 @@
         <v>67</v>
       </c>
       <c r="E41" s="33" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F41" s="67" t="s">
         <v>93</v>
       </c>
       <c r="G41" s="67" t="s">
+        <v>114</v>
+      </c>
+      <c r="H41" s="68" t="s">
         <v>115</v>
-      </c>
-      <c r="H41" s="68" t="s">
-        <v>116</v>
       </c>
       <c r="I41" s="69" t="s">
         <v>11</v>
       </c>
       <c r="J41" s="69"/>
       <c r="K41" s="70" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="42" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -4452,23 +4452,23 @@
         <v>67</v>
       </c>
       <c r="E42" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F42" s="71" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G42" s="71" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H42" s="72" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I42" s="71" t="s">
         <v>11</v>
       </c>
       <c r="J42" s="71"/>
       <c r="K42" s="65" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -4491,29 +4491,29 @@
         <v>Contact.contactIdentifier</v>
       </c>
       <c r="C44" s="21" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D44" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E44" s="33" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F44" s="78" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="G44" s="78" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H44" s="79" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="I44" s="26" t="s">
         <v>11</v>
       </c>
       <c r="J44" s="26"/>
       <c r="K44" s="65" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -4523,29 +4523,29 @@
         <v>Contact.emailAddress</v>
       </c>
       <c r="C45" s="21" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D45" s="66" t="s">
         <v>67</v>
       </c>
       <c r="E45" s="33" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F45" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="G45" s="43" t="s">
+        <v>150</v>
+      </c>
+      <c r="H45" s="80" t="s">
         <v>151</v>
-      </c>
-      <c r="G45" s="43" t="s">
-        <v>152</v>
-      </c>
-      <c r="H45" s="80" t="s">
-        <v>153</v>
       </c>
       <c r="I45" s="26" t="s">
         <v>11</v>
       </c>
       <c r="J45" s="26"/>
       <c r="K45" s="27" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -4555,29 +4555,29 @@
         <v>Contact.phoneNumber</v>
       </c>
       <c r="C46" s="21" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D46" s="66" t="s">
         <v>67</v>
       </c>
       <c r="E46" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F46" s="43" t="s">
+        <v>152</v>
+      </c>
+      <c r="G46" s="43" t="s">
+        <v>153</v>
+      </c>
+      <c r="H46" s="44" t="s">
         <v>154</v>
-      </c>
-      <c r="G46" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="H46" s="44" t="s">
-        <v>156</v>
       </c>
       <c r="I46" s="26" t="s">
         <v>11</v>
       </c>
       <c r="J46" s="26"/>
       <c r="K46" s="27" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -4587,29 +4587,29 @@
         <v>Contact.firstName</v>
       </c>
       <c r="C47" s="21" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D47" s="66" t="s">
         <v>67</v>
       </c>
       <c r="E47" s="33" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F47" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="G47" s="43" t="s">
+        <v>156</v>
+      </c>
+      <c r="H47" s="44" t="s">
         <v>157</v>
-      </c>
-      <c r="G47" s="43" t="s">
-        <v>158</v>
-      </c>
-      <c r="H47" s="44" t="s">
-        <v>159</v>
       </c>
       <c r="I47" s="26" t="s">
         <v>11</v>
       </c>
       <c r="J47" s="26"/>
       <c r="K47" s="27" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -4619,29 +4619,29 @@
         <v>Contact.lastName</v>
       </c>
       <c r="C48" s="21" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D48" s="66" t="s">
         <v>67</v>
       </c>
       <c r="E48" s="33" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F48" s="43" t="s">
+        <v>158</v>
+      </c>
+      <c r="G48" s="43" t="s">
+        <v>159</v>
+      </c>
+      <c r="H48" s="81" t="s">
         <v>160</v>
-      </c>
-      <c r="G48" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="H48" s="81" t="s">
-        <v>162</v>
       </c>
       <c r="I48" s="26" t="s">
         <v>11</v>
       </c>
       <c r="J48" s="26"/>
       <c r="K48" s="27" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="49" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -4651,29 +4651,29 @@
         <v>Contact.faxNumber</v>
       </c>
       <c r="C49" s="21" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D49" s="66" t="s">
         <v>67</v>
       </c>
       <c r="E49" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F49" s="43" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G49" s="43" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H49" s="44" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="I49" s="26" t="s">
         <v>11</v>
       </c>
       <c r="J49" s="26"/>
       <c r="K49" s="27" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -4683,29 +4683,29 @@
         <v>Contact.locale</v>
       </c>
       <c r="C50" s="21" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D50" s="66" t="s">
         <v>67</v>
       </c>
       <c r="E50" s="33" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="F50" s="43" t="s">
+        <v>163</v>
+      </c>
+      <c r="G50" s="43" t="s">
+        <v>164</v>
+      </c>
+      <c r="H50" s="44" t="s">
         <v>165</v>
-      </c>
-      <c r="G50" s="43" t="s">
-        <v>166</v>
-      </c>
-      <c r="H50" s="44" t="s">
-        <v>167</v>
       </c>
       <c r="I50" s="26" t="s">
         <v>11</v>
       </c>
       <c r="J50" s="26"/>
       <c r="K50" s="27" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="51" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -4734,7 +4734,7 @@
         <v>8</v>
       </c>
       <c r="E52" s="23" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F52" s="24" t="s">
         <v>9</v>
@@ -4750,7 +4750,7 @@
       </c>
       <c r="J52" s="26"/>
       <c r="K52" s="27" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -4766,7 +4766,7 @@
         <v>8</v>
       </c>
       <c r="E53" s="23" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F53" s="28" t="s">
         <v>12</v>
@@ -4775,14 +4775,14 @@
         <v>13</v>
       </c>
       <c r="H53" s="30" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I53" s="26" t="s">
         <v>11</v>
       </c>
       <c r="J53" s="26"/>
       <c r="K53" s="31" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="54" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -4798,7 +4798,7 @@
         <v>14</v>
       </c>
       <c r="E54" s="33" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="F54" s="34" t="s">
         <v>15</v>
@@ -4814,7 +4814,7 @@
       </c>
       <c r="J54" s="36"/>
       <c r="K54" s="27" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="55" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -4830,7 +4830,7 @@
         <v>18</v>
       </c>
       <c r="E55" s="23" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F55" s="38" t="s">
         <v>19</v>
@@ -4845,10 +4845,10 @@
         <v>22</v>
       </c>
       <c r="J55" s="40" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="K55" s="27" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -4864,7 +4864,7 @@
         <v>18</v>
       </c>
       <c r="E56" s="23" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F56" s="38" t="s">
         <v>23</v>
@@ -4879,10 +4879,10 @@
         <v>22</v>
       </c>
       <c r="J56" s="40" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="K56" s="27" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
@@ -4898,7 +4898,7 @@
         <v>18</v>
       </c>
       <c r="E57" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F57" s="38" t="s">
         <v>26</v>
@@ -4913,10 +4913,10 @@
         <v>22</v>
       </c>
       <c r="J57" s="41" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="K57" s="27" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
@@ -4932,7 +4932,7 @@
         <v>18</v>
       </c>
       <c r="E58" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F58" s="38" t="s">
         <v>28</v>
@@ -4947,10 +4947,10 @@
         <v>22</v>
       </c>
       <c r="J58" s="41" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="K58" s="27" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
@@ -4966,7 +4966,7 @@
         <v>34</v>
       </c>
       <c r="E59" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F59" s="43" t="s">
         <v>35</v>
@@ -4982,7 +4982,7 @@
       </c>
       <c r="J59" s="45"/>
       <c r="K59" s="46" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -4998,7 +4998,7 @@
         <v>38</v>
       </c>
       <c r="E60" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F60" s="43" t="s">
         <v>39</v>
@@ -5007,14 +5007,14 @@
         <v>40</v>
       </c>
       <c r="H60" s="44" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="I60" s="45" t="s">
         <v>41</v>
       </c>
       <c r="J60" s="45"/>
       <c r="K60" s="46" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -5030,7 +5030,7 @@
         <v>38</v>
       </c>
       <c r="E61" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F61" s="43" t="s">
         <v>42</v>
@@ -5039,14 +5039,14 @@
         <v>43</v>
       </c>
       <c r="H61" s="48" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="I61" s="45" t="s">
         <v>41</v>
       </c>
       <c r="J61" s="45"/>
       <c r="K61" s="46" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
@@ -5062,7 +5062,7 @@
         <v>38</v>
       </c>
       <c r="E62" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F62" s="43" t="s">
         <v>44</v>
@@ -5071,14 +5071,14 @@
         <v>45</v>
       </c>
       <c r="H62" s="44" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="I62" s="45" t="s">
         <v>41</v>
       </c>
       <c r="J62" s="45"/>
       <c r="K62" s="46" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
@@ -5094,7 +5094,7 @@
         <v>38</v>
       </c>
       <c r="E63" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F63" s="43" t="s">
         <v>46</v>
@@ -5103,14 +5103,14 @@
         <v>47</v>
       </c>
       <c r="H63" s="44" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="I63" s="45" t="s">
         <v>41</v>
       </c>
       <c r="J63" s="45"/>
       <c r="K63" s="46" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
@@ -5126,7 +5126,7 @@
         <v>38</v>
       </c>
       <c r="E64" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F64" s="43" t="s">
         <v>48</v>
@@ -5135,14 +5135,14 @@
         <v>49</v>
       </c>
       <c r="H64" s="44" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="I64" s="45" t="s">
         <v>41</v>
       </c>
       <c r="J64" s="45"/>
       <c r="K64" s="46" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="65" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -5158,7 +5158,7 @@
         <v>50</v>
       </c>
       <c r="E65" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F65" s="43" t="s">
         <v>51</v>
@@ -5174,7 +5174,7 @@
       </c>
       <c r="J65" s="45"/>
       <c r="K65" s="27" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
@@ -5190,7 +5190,7 @@
         <v>50</v>
       </c>
       <c r="E66" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F66" s="43" t="s">
         <v>54</v>
@@ -5206,7 +5206,7 @@
       </c>
       <c r="J66" s="45"/>
       <c r="K66" s="46" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
@@ -5222,7 +5222,7 @@
         <v>50</v>
       </c>
       <c r="E67" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F67" s="43" t="s">
         <v>57</v>
@@ -5238,7 +5238,7 @@
       </c>
       <c r="J67" s="45"/>
       <c r="K67" s="27" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
@@ -5254,7 +5254,7 @@
         <v>50</v>
       </c>
       <c r="E68" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F68" s="43" t="s">
         <v>59</v>
@@ -5270,7 +5270,7 @@
       </c>
       <c r="J68" s="45"/>
       <c r="K68" s="46" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
@@ -5286,7 +5286,7 @@
         <v>50</v>
       </c>
       <c r="E69" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F69" s="50" t="s">
         <v>62</v>
@@ -5302,7 +5302,7 @@
       </c>
       <c r="J69" s="45"/>
       <c r="K69" s="51" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="70" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -5318,7 +5318,7 @@
         <v>50</v>
       </c>
       <c r="E70" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F70" s="43" t="s">
         <v>65</v>
@@ -5334,7 +5334,7 @@
       </c>
       <c r="J70" s="45"/>
       <c r="K70" s="27" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="71" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -5363,7 +5363,7 @@
         <v>8</v>
       </c>
       <c r="E72" s="52" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F72" s="53" t="s">
         <v>69</v>
@@ -5378,10 +5378,10 @@
         <v>22</v>
       </c>
       <c r="J72" s="53" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="K72" s="27" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
@@ -5397,7 +5397,7 @@
         <v>8</v>
       </c>
       <c r="E73" s="52" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F73" s="24" t="s">
         <v>70</v>
@@ -5413,7 +5413,7 @@
       </c>
       <c r="J73" s="26"/>
       <c r="K73" s="46" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
@@ -5429,7 +5429,7 @@
         <v>8</v>
       </c>
       <c r="E74" s="52" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F74" s="53" t="s">
         <v>72</v>
@@ -5438,16 +5438,16 @@
         <v>13</v>
       </c>
       <c r="H74" s="54" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I74" s="53" t="s">
         <v>22</v>
       </c>
       <c r="J74" s="53" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="K74" s="31" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
@@ -5463,7 +5463,7 @@
         <v>18</v>
       </c>
       <c r="E75" s="33" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F75" s="38" t="s">
         <v>73</v>
@@ -5478,10 +5478,10 @@
         <v>22</v>
       </c>
       <c r="J75" s="38" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="K75" s="27" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
@@ -5497,7 +5497,7 @@
         <v>18</v>
       </c>
       <c r="E76" s="33" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F76" s="38" t="s">
         <v>28</v>
@@ -5512,10 +5512,10 @@
         <v>22</v>
       </c>
       <c r="J76" s="41" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="K76" s="27" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
@@ -5531,7 +5531,7 @@
         <v>18</v>
       </c>
       <c r="E77" s="33" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F77" s="38" t="s">
         <v>26</v>
@@ -5546,10 +5546,10 @@
         <v>22</v>
       </c>
       <c r="J77" s="41" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="K77" s="27" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
@@ -5565,7 +5565,7 @@
         <v>34</v>
       </c>
       <c r="E78" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F78" s="43" t="s">
         <v>77</v>
@@ -5581,7 +5581,7 @@
       </c>
       <c r="J78" s="45"/>
       <c r="K78" s="27" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
@@ -5597,7 +5597,7 @@
         <v>38</v>
       </c>
       <c r="E79" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F79" s="43" t="s">
         <v>39</v>
@@ -5606,14 +5606,14 @@
         <v>40</v>
       </c>
       <c r="H79" s="44" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="I79" s="45" t="s">
         <v>41</v>
       </c>
       <c r="J79" s="45"/>
       <c r="K79" s="46" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
@@ -5629,7 +5629,7 @@
         <v>38</v>
       </c>
       <c r="E80" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F80" s="56" t="s">
         <v>42</v>
@@ -5638,14 +5638,14 @@
         <v>43</v>
       </c>
       <c r="H80" s="44" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="I80" s="45" t="s">
         <v>41</v>
       </c>
       <c r="J80" s="45"/>
       <c r="K80" s="46" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="81" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -5661,7 +5661,7 @@
         <v>38</v>
       </c>
       <c r="E81" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F81" s="56" t="s">
         <v>44</v>
@@ -5670,14 +5670,14 @@
         <v>45</v>
       </c>
       <c r="H81" s="44" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="I81" s="45" t="s">
         <v>41</v>
       </c>
       <c r="J81" s="45"/>
       <c r="K81" s="46" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="82" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -5693,7 +5693,7 @@
         <v>38</v>
       </c>
       <c r="E82" s="33" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F82" s="43" t="s">
         <v>46</v>
@@ -5702,14 +5702,14 @@
         <v>47</v>
       </c>
       <c r="H82" s="44" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="I82" s="45" t="s">
         <v>41</v>
       </c>
       <c r="J82" s="45"/>
       <c r="K82" s="46" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
@@ -5725,7 +5725,7 @@
         <v>38</v>
       </c>
       <c r="E83" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F83" s="43" t="s">
         <v>48</v>
@@ -5734,14 +5734,14 @@
         <v>49</v>
       </c>
       <c r="H83" s="44" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="I83" s="45" t="s">
         <v>41</v>
       </c>
       <c r="J83" s="45"/>
       <c r="K83" s="46" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="84" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -5757,7 +5757,7 @@
         <v>50</v>
       </c>
       <c r="E84" s="33" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F84" s="43" t="s">
         <v>51</v>
@@ -5773,7 +5773,7 @@
       </c>
       <c r="J84" s="45"/>
       <c r="K84" s="27" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
@@ -5789,7 +5789,7 @@
         <v>50</v>
       </c>
       <c r="E85" s="33" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F85" s="43" t="s">
         <v>54</v>
@@ -5805,7 +5805,7 @@
       </c>
       <c r="J85" s="45"/>
       <c r="K85" s="46" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="86" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -5821,7 +5821,7 @@
         <v>50</v>
       </c>
       <c r="E86" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F86" s="43" t="s">
         <v>81</v>
@@ -5838,7 +5838,7 @@
       </c>
       <c r="J86" s="45"/>
       <c r="K86" s="27" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="87" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -5854,7 +5854,7 @@
         <v>50</v>
       </c>
       <c r="E87" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F87" s="43" t="s">
         <v>83</v>
@@ -5870,7 +5870,7 @@
       </c>
       <c r="J87" s="45"/>
       <c r="K87" s="27" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
@@ -5886,7 +5886,7 @@
         <v>50</v>
       </c>
       <c r="E88" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F88" s="43" t="s">
         <v>84</v>
@@ -5902,7 +5902,7 @@
       </c>
       <c r="J88" s="45"/>
       <c r="K88" s="46" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="89" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -5918,7 +5918,7 @@
         <v>50</v>
       </c>
       <c r="E89" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F89" s="50" t="s">
         <v>85</v>
@@ -5934,7 +5934,7 @@
       </c>
       <c r="J89" s="45"/>
       <c r="K89" s="27" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update templates and data dictionary
</commit_message>
<xml_diff>
--- a/Envizi-SCI Data Dictionary (simplified).xlsx
+++ b/Envizi-SCI Data Dictionary (simplified).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\903106897\Box\Sustainability Platform\2.4 Products - implementation\5. Content drafts\5. Configuring\E-SCI-data-templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MikeWhitney\Box\Sustainability Platform\2.2 Products - PM\1 - Scope 3.1\7 - Docs and training\E-SCI data dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D3BA35-0682-4BEC-BBF1-CCE11FC6ADFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997159BF-F768-4574-9007-F9AC72954B7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6675" yWindow="2355" windowWidth="33540" windowHeight="24495" tabRatio="763" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6150" yWindow="6150" windowWidth="25845" windowHeight="21780" tabRatio="763" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data summary" sheetId="31" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Import data dictionary'!$A$1:$K$50</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -1753,13 +1754,13 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
     <mruColors>
+      <color rgb="FFFFCCFF"/>
       <color rgb="FFFFFF99"/>
       <color rgb="FFF9C7F7"/>
       <color rgb="FFFFE7FF"/>
       <color rgb="FF6A619D"/>
       <color rgb="FF3391CB"/>
       <color rgb="FFF6B0F3"/>
-      <color rgb="FFFFCCFF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -3169,8 +3170,8 @@
   <dimension ref="A1:K89"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H27" sqref="H27"/>
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5854,7 +5855,7 @@
         <v>50</v>
       </c>
       <c r="E87" s="33" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F87" s="43" t="s">
         <v>83</v>
@@ -5886,7 +5887,7 @@
         <v>50</v>
       </c>
       <c r="E88" s="33" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F88" s="43" t="s">
         <v>84</v>

</xml_diff>